<commit_message>
Refactoring code to allow a more flexible definition of variables, including nested filtering on multiple categories. Still minor issue on filtering intra-problem sets (will solve in next commits).
</commit_message>
<xml_diff>
--- a/tests/fixtures/variables_new_cat/sets.xlsx
+++ b/tests/fixtures/variables_new_cat/sets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\fixtures\variables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\fixtures\variables_new_cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A88E9F-6A81-45B6-ADD9-47EC2E2B9E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5674D0E-94D0-4A1F-8C75-6E53A14E9EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16180" yWindow="2730" windowWidth="15360" windowHeight="15370" tabRatio="757" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19930" yWindow="2870" windowWidth="15360" windowHeight="15370" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_set_CASES" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>c_Name</t>
   </si>
@@ -32,22 +32,28 @@
     <t>y_Name</t>
   </si>
   <si>
+    <t>y_Category_1</t>
+  </si>
+  <si>
     <t>t_Name</t>
   </si>
   <si>
-    <t>t_Category</t>
+    <t>t_Category_1</t>
+  </si>
+  <si>
+    <t>t_Category_2</t>
   </si>
   <si>
     <t>f_Name</t>
   </si>
   <si>
-    <t>f_Category</t>
+    <t>f_Category_1</t>
   </si>
   <si>
     <t>f_agg_Name</t>
   </si>
   <si>
-    <t>base</t>
+    <t>baseline</t>
   </si>
   <si>
     <t>y.1</t>
@@ -68,6 +74,24 @@
     <t>y.6</t>
   </si>
   <si>
+    <t>y.7</t>
+  </si>
+  <si>
+    <t>y.8</t>
+  </si>
+  <si>
+    <t>y.9</t>
+  </si>
+  <si>
+    <t>y.10</t>
+  </si>
+  <si>
+    <t>warm-up</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
     <t>fossil fuels plant</t>
   </si>
   <si>
@@ -83,28 +107,37 @@
     <t>govern</t>
   </si>
   <si>
-    <t>Supply technology</t>
-  </si>
-  <si>
-    <t>Demand technology</t>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Non-Renewable</t>
+  </si>
+  <si>
+    <t>Renewable</t>
+  </si>
+  <si>
+    <t>Elon-Musk-Approved</t>
   </si>
   <si>
     <t>power by fossil</t>
   </si>
   <si>
+    <t>electricity</t>
+  </si>
+  <si>
     <t>power by res</t>
   </si>
   <si>
     <t>oil products</t>
   </si>
   <si>
-    <t>physical flow</t>
-  </si>
-  <si>
-    <t>economic flow</t>
-  </si>
-  <si>
-    <t>electricity</t>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Economic</t>
   </si>
   <si>
     <t>f_agg_Category</t>
@@ -479,7 +512,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J46" sqref="J45:J46"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,7 +524,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -501,47 +534,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -552,63 +638,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -621,53 +723,53 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -680,33 +782,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>